<commit_message>
Conduct S3 tests for Graphql with resolved fields
</commit_message>
<xml_diff>
--- a/Wyniki 3/S1/S1-GraphQL — jedno pole — zoptymalizowane.xlsx
+++ b/Wyniki 3/S1/S1-GraphQL — jedno pole — zoptymalizowane.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\S1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B27B166-4BF2-41DF-94E8-AF8C4E88A22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD06FA9-0320-4675-80A2-4CA90D91D873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 rekord" sheetId="1" r:id="rId1"/>
     <sheet name="100 rekordów" sheetId="2" r:id="rId2"/>
     <sheet name="500 rekordów" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -765,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -794,9 +805,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1079,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E7:K38"/>
+  <dimension ref="E7:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1099,7 @@
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1102,7 +1110,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,11 +1129,11 @@
       <c r="J8" s="1">
         <v>4</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" s="7">
         <v>100</v>
       </c>
@@ -1144,11 +1152,11 @@
       <c r="J9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="1" t="s">
         <v>2</v>
@@ -1165,11 +1173,11 @@
       <c r="J10" s="6">
         <v>0</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
@@ -1186,11 +1194,11 @@
       <c r="J11" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
@@ -1207,11 +1215,11 @@
       <c r="J12" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
         <v>5</v>
@@ -1228,11 +1236,11 @@
       <c r="J13" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
         <v>6</v>
@@ -1249,11 +1257,15 @@
       <c r="J14" s="6">
         <v>83931</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="1">
         <v>83930</v>
       </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f>AVERAGE(G14:K14)</f>
+        <v>83929.4</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1270,11 +1282,15 @@
       <c r="J15" s="6">
         <v>960.2</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="1">
         <v>960.2</v>
       </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" ref="L15:L38" si="0">AVERAGE(G15:K15)</f>
+        <v>960.16000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1291,11 +1307,15 @@
       <c r="J16" s="6">
         <v>87.41</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="1">
         <v>87.41</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>87.411999999999992</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="7"/>
       <c r="F17" s="1" t="s">
         <v>9</v>
@@ -1312,11 +1332,15 @@
       <c r="J17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="7"/>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -1333,11 +1357,15 @@
       <c r="J18" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="8">
         <v>1000</v>
       </c>
@@ -1359,8 +1387,12 @@
       <c r="K19" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="8"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
@@ -1380,8 +1412,12 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" s="8"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
@@ -1401,8 +1437,12 @@
       <c r="K21" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22" s="8"/>
       <c r="F22" s="2" t="s">
         <v>4</v>
@@ -1422,8 +1462,12 @@
       <c r="K22" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23" s="8"/>
       <c r="F23" s="2" t="s">
         <v>5</v>
@@ -1443,8 +1487,12 @@
       <c r="K23" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24" s="8"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
@@ -1464,8 +1512,12 @@
       <c r="K24" s="4">
         <v>839200</v>
       </c>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>839198.6</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" s="8"/>
       <c r="F25" s="2" t="s">
         <v>7</v>
@@ -1485,8 +1537,12 @@
       <c r="K25" s="4">
         <v>960.6</v>
       </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>960.62000000000012</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" s="8"/>
       <c r="F26" s="2" t="s">
         <v>8</v>
@@ -1506,8 +1562,12 @@
       <c r="K26" s="4">
         <v>873.63</v>
       </c>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>873.61199999999985</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" s="8"/>
       <c r="F27" s="2" t="s">
         <v>9</v>
@@ -1527,8 +1587,12 @@
       <c r="K27" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28" s="8"/>
       <c r="F28" s="2" t="s">
         <v>10</v>
@@ -1548,8 +1612,12 @@
       <c r="K28" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" s="7">
         <v>4000</v>
       </c>
@@ -1571,8 +1639,12 @@
       <c r="K29" s="6" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" s="7"/>
       <c r="F30" s="1" t="s">
         <v>2</v>
@@ -1592,8 +1664,12 @@
       <c r="K30" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" s="7"/>
       <c r="F31" s="1" t="s">
         <v>3</v>
@@ -1613,8 +1689,12 @@
       <c r="K31" s="6" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32" s="7"/>
       <c r="F32" s="1" t="s">
         <v>4</v>
@@ -1634,8 +1714,12 @@
       <c r="K32" s="6" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" s="7"/>
       <c r="F33" s="1" t="s">
         <v>5</v>
@@ -1655,8 +1739,12 @@
       <c r="K33" s="6" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" s="7"/>
       <c r="F34" s="1" t="s">
         <v>6</v>
@@ -1676,8 +1764,12 @@
       <c r="K34" s="6">
         <v>2375413</v>
       </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>2371057</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" s="7"/>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -1697,8 +1789,12 @@
       <c r="K35" s="6">
         <v>960.6</v>
       </c>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>960.58000000000015</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" s="7"/>
       <c r="F36" s="1" t="s">
         <v>8</v>
@@ -1718,8 +1814,12 @@
       <c r="K36" s="6">
         <v>2472.84</v>
       </c>
-    </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>2468.364</v>
+      </c>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E37" s="7"/>
       <c r="F37" s="1" t="s">
         <v>9</v>
@@ -1739,8 +1839,12 @@
       <c r="K37" s="6" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" s="7"/>
       <c r="F38" s="1" t="s">
         <v>10</v>
@@ -1759,6 +1863,10 @@
       </c>
       <c r="K38" s="6" t="s">
         <v>214</v>
+      </c>
+      <c r="L38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1774,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4FD128-804F-4FC8-966B-DED231E7146F}">
-  <dimension ref="E7:K38"/>
+  <dimension ref="E7:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1894,7 @@
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1905,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1813,14 +1921,14 @@
       <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="1">
         <v>4</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E9" s="7">
         <v>100</v>
       </c>
@@ -1836,14 +1944,14 @@
       <c r="I9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="1" t="s">
         <v>2</v>
@@ -1857,14 +1965,14 @@
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="12">
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="1" t="s">
         <v>3</v>
@@ -1878,14 +1986,14 @@
       <c r="I11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="1" t="s">
         <v>4</v>
@@ -1899,14 +2007,14 @@
       <c r="I12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="1" t="s">
         <v>5</v>
@@ -1920,14 +2028,14 @@
       <c r="I13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="1" t="s">
         <v>6</v>
@@ -1941,14 +2049,18 @@
       <c r="I14" s="1">
         <v>83930</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="1">
         <v>83937</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="1">
         <v>83931</v>
       </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f>AVERAGE(G14:K14)</f>
+        <v>83932</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="1" t="s">
         <v>7</v>
@@ -1962,14 +2074,18 @@
       <c r="I15" s="1">
         <v>961</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="1">
         <v>960</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="1">
         <v>960.1</v>
       </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" ref="L15:L38" si="0">AVERAGE(G15:K15)</f>
+        <v>960.7</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -1983,14 +2099,18 @@
       <c r="I16" s="1">
         <v>87.34</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="1">
         <v>87.43</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="1">
         <v>87.42</v>
       </c>
-    </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>87.366000000000014</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="7"/>
       <c r="F17" s="1" t="s">
         <v>13</v>
@@ -2004,14 +2124,18 @@
       <c r="I17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="7"/>
       <c r="F18" s="1" t="s">
         <v>10</v>
@@ -2025,14 +2149,18 @@
       <c r="I18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="J18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="8">
         <v>1000</v>
       </c>
@@ -2054,8 +2182,12 @@
       <c r="K19" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="8"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
@@ -2075,8 +2207,12 @@
       <c r="K20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" s="8"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
@@ -2096,8 +2232,12 @@
       <c r="K21" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E22" s="8"/>
       <c r="F22" s="2" t="s">
         <v>4</v>
@@ -2117,8 +2257,12 @@
       <c r="K22" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E23" s="8"/>
       <c r="F23" s="2" t="s">
         <v>5</v>
@@ -2138,8 +2282,12 @@
       <c r="K23" s="5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E24" s="8"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
@@ -2159,8 +2307,12 @@
       <c r="K24" s="5">
         <v>839106</v>
       </c>
-    </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>839034.4</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E25" s="8"/>
       <c r="F25" s="2" t="s">
         <v>7</v>
@@ -2180,8 +2332,12 @@
       <c r="K25" s="5">
         <v>960.8</v>
       </c>
-    </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>960.8</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E26" s="8"/>
       <c r="F26" s="2" t="s">
         <v>8</v>
@@ -2201,8 +2357,12 @@
       <c r="K26" s="5">
         <v>873.32</v>
       </c>
-    </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>873.2700000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E27" s="8"/>
       <c r="F27" s="2" t="s">
         <v>13</v>
@@ -2222,8 +2382,12 @@
       <c r="K27" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E28" s="8"/>
       <c r="F28" s="2" t="s">
         <v>10</v>
@@ -2243,8 +2407,12 @@
       <c r="K28" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E29" s="7">
         <v>4000</v>
       </c>
@@ -2266,8 +2434,12 @@
       <c r="K29" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" s="7"/>
       <c r="F30" s="1" t="s">
         <v>2</v>
@@ -2287,8 +2459,12 @@
       <c r="K30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E31" s="7"/>
       <c r="F31" s="1" t="s">
         <v>3</v>
@@ -2308,8 +2484,12 @@
       <c r="K31" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E32" s="7"/>
       <c r="F32" s="1" t="s">
         <v>4</v>
@@ -2329,8 +2509,12 @@
       <c r="K32" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" s="7"/>
       <c r="F33" s="1" t="s">
         <v>5</v>
@@ -2350,8 +2534,12 @@
       <c r="K33" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" s="7"/>
       <c r="F34" s="1" t="s">
         <v>6</v>
@@ -2371,8 +2559,12 @@
       <c r="K34" s="3">
         <v>1626401</v>
       </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>1639046.2</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" s="7"/>
       <c r="F35" s="1" t="s">
         <v>7</v>
@@ -2392,8 +2584,12 @@
       <c r="K35" s="3">
         <v>960.7</v>
       </c>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>960.75999999999988</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" s="7"/>
       <c r="F36" s="1" t="s">
         <v>8</v>
@@ -2413,8 +2609,12 @@
       <c r="K36" s="3">
         <v>1692.88</v>
       </c>
-    </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>1706.002</v>
+      </c>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E37" s="7"/>
       <c r="F37" s="1" t="s">
         <v>13</v>
@@ -2434,8 +2634,12 @@
       <c r="K37" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" s="7"/>
       <c r="F38" s="1" t="s">
         <v>10</v>
@@ -2454,6 +2658,10 @@
       </c>
       <c r="K38" s="3" t="s">
         <v>152</v>
+      </c>
+      <c r="L38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -2471,8 +2679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5008BA1D-A9B8-490D-8D36-2848B9455033}">
   <dimension ref="E7:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,6 +2895,10 @@
       <c r="K14" s="6">
         <v>83915</v>
       </c>
+      <c r="L14">
+        <f>AVERAGE(G14:K14)</f>
+        <v>83915</v>
+      </c>
       <c r="N14" s="1">
         <v>83752</v>
       </c>
@@ -2717,6 +2929,10 @@
       <c r="K15" s="6">
         <v>960.2</v>
       </c>
+      <c r="L15">
+        <f t="shared" ref="L15:L38" si="0">AVERAGE(G15:K15)</f>
+        <v>960.21999999999991</v>
+      </c>
       <c r="N15" s="1">
         <v>960.1</v>
       </c>
@@ -2747,6 +2963,10 @@
       <c r="K16" s="6">
         <v>87.39</v>
       </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>87.387999999999991</v>
+      </c>
       <c r="N16" s="1">
         <v>87.23</v>
       </c>
@@ -2777,6 +2997,10 @@
       <c r="K17" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="L17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2807,6 +3031,10 @@
       <c r="K18" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="L18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2838,6 +3066,10 @@
       </c>
       <c r="K19" s="4" t="s">
         <v>73</v>
+      </c>
+      <c r="L19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="N19" s="2">
         <v>1990</v>
@@ -2869,6 +3101,10 @@
       <c r="K20" s="4">
         <v>0</v>
       </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2899,6 +3135,10 @@
       <c r="K21" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="L21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N21" s="2">
         <v>2600</v>
       </c>
@@ -2929,6 +3169,10 @@
       <c r="K22" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="L22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N22" s="2">
         <v>2310</v>
       </c>
@@ -2959,6 +3203,10 @@
       <c r="K23" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>657.53</v>
+      </c>
       <c r="N23" s="2">
         <v>2330</v>
       </c>
@@ -2989,6 +3237,10 @@
       <c r="K24" s="4">
         <v>549661</v>
       </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>548493.6</v>
+      </c>
       <c r="N24" s="2">
         <v>280441</v>
       </c>
@@ -3019,6 +3271,10 @@
       <c r="K25" s="4">
         <v>960.9</v>
       </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>960.7</v>
+      </c>
       <c r="N25" s="2">
         <v>960.5</v>
       </c>
@@ -3049,6 +3305,10 @@
       <c r="K26" s="4">
         <v>572.04</v>
       </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>570.92600000000004</v>
+      </c>
       <c r="N26" s="2">
         <v>291.97000000000003</v>
       </c>
@@ -3079,6 +3339,10 @@
       <c r="K27" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="L27" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3109,6 +3373,10 @@
       <c r="K28" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="L28" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N28" s="2" t="s">
         <v>24</v>
       </c>
@@ -3140,6 +3408,10 @@
       </c>
       <c r="K29" s="6" t="s">
         <v>83</v>
+      </c>
+      <c r="L29" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="N29" s="1">
         <v>10820</v>
@@ -3171,6 +3443,10 @@
       <c r="K30" s="6">
         <v>0</v>
       </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N30" s="1" t="s">
         <v>16</v>
       </c>
@@ -3201,6 +3477,10 @@
       <c r="K31" s="6" t="s">
         <v>91</v>
       </c>
+      <c r="L31" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N31" s="1">
         <v>12600</v>
       </c>
@@ -3231,6 +3511,10 @@
       <c r="K32" s="6" t="s">
         <v>85</v>
       </c>
+      <c r="L32" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N32" s="1">
         <v>12400</v>
       </c>
@@ -3261,6 +3545,10 @@
       <c r="K33" s="6" t="s">
         <v>86</v>
       </c>
+      <c r="L33" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N33" s="1">
         <v>12420</v>
       </c>
@@ -3291,6 +3579,10 @@
       <c r="K34" s="6">
         <v>580469</v>
       </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>580370.19999999995</v>
+      </c>
       <c r="N34" s="1">
         <v>285420</v>
       </c>
@@ -3321,6 +3613,10 @@
       <c r="K35" s="6">
         <v>960.5</v>
       </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>960.74000000000012</v>
+      </c>
       <c r="N35" s="1">
         <v>960.8</v>
       </c>
@@ -3351,6 +3647,10 @@
       <c r="K36" s="6">
         <v>604.35</v>
       </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>604.09399999999994</v>
+      </c>
       <c r="N36" s="1">
         <v>297.07</v>
       </c>
@@ -3381,6 +3681,10 @@
       <c r="K37" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="L37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N37" s="1">
         <v>2.8</v>
       </c>
@@ -3410,6 +3714,10 @@
       </c>
       <c r="K38" s="6" t="s">
         <v>82</v>
+      </c>
+      <c r="L38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="N38" s="1">
         <v>89</v>

</xml_diff>